<commit_message>
-Decomposed the original simulation into multiple functions. -All of the functions have been tested and seem to work. -The simulation structure is mostly done except for the acquiring infections (mixing)
TODO:
1) modify find_demog_indices to work for everything instead of just demographics
2) clarify valid transitions and correct order of transitions and then code them
3) documentation
4) scripts to produce input csv files
</commit_message>
<xml_diff>
--- a/doc/feature_codebook.xlsx
+++ b/doc/feature_codebook.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michellezhao/Desktop/github/hiv_simulation/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michellezhao/Desktop/github/hiv_simulation/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{49724B65-6C51-D843-B64F-D7E82044681D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BDFC8E29-A4E5-914D-A899-B10F7D54CF98}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10500" windowWidth="16800" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feature_codebook" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>variable_name</t>
   </si>
@@ -58,24 +58,12 @@
     <t>men who have sex with men</t>
   </si>
   <si>
-    <t>IDU</t>
-  </si>
-  <si>
-    <t>injection drug user</t>
-  </si>
-  <si>
     <t>alive</t>
   </si>
   <si>
     <t>alive in the current time period</t>
   </si>
   <si>
-    <t>in_simulation</t>
-  </si>
-  <si>
-    <t>currently active in the simulation whether dead or alive</t>
-  </si>
-  <si>
     <t>categorical</t>
   </si>
   <si>
@@ -91,42 +79,18 @@
     <t>AIDS</t>
   </si>
   <si>
-    <t>MMT</t>
-  </si>
-  <si>
-    <t>on MMT (methadone maintenance treatment)</t>
-  </si>
-  <si>
     <t>PrEP</t>
   </si>
   <si>
-    <t>on PrEP (pre-exposure prophylaxis)</t>
-  </si>
-  <si>
     <t>ART</t>
   </si>
   <si>
-    <t>on ART (anti-retroviral therapy)</t>
-  </si>
-  <si>
     <t>HIV</t>
   </si>
   <si>
     <t>race</t>
   </si>
   <si>
-    <t>incarceration</t>
-  </si>
-  <si>
-    <t>never incarcerated</t>
-  </si>
-  <si>
-    <t>currently incarcerated</t>
-  </si>
-  <si>
-    <t>has been incarcerated previously</t>
-  </si>
-  <si>
     <t>white</t>
   </si>
   <si>
@@ -140,6 +104,24 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>not on ART (anti-retroviral therapy)</t>
+  </si>
+  <si>
+    <t>on ART, adherent</t>
+  </si>
+  <si>
+    <t>was on ART, not adherent</t>
+  </si>
+  <si>
+    <t>not on PrEP (pre-exposure prophylaxis)</t>
+  </si>
+  <si>
+    <t>on PrEP, adherent</t>
+  </si>
+  <si>
+    <t>on PrEP, not adherent</t>
   </si>
 </sst>
 </file>
@@ -980,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="102" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1024,16 +1006,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1041,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1049,7 +1031,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1057,7 +1039,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1065,173 +1047,133 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
         <v>18</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
-        <v>10</v>
+      <c r="C15">
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
       <c r="C18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
+      <c r="C20">
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified feature codebook to reflect the drabo simulation
</commit_message>
<xml_diff>
--- a/doc/feature_codebook.xlsx
+++ b/doc/feature_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michellezhao/Desktop/github/hiv_simulation/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BDFC8E29-A4E5-914D-A899-B10F7D54CF98}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60276F3B-FCC5-D643-A057-81649F98129D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10500" windowWidth="16800" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20460" yWindow="260" windowWidth="16800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feature_codebook" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>variable_name</t>
   </si>
@@ -34,21 +34,12 @@
     <t>description</t>
   </si>
   <si>
-    <t>age</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
     <t>0-100</t>
   </si>
   <si>
-    <t>age of person rounded to nearest integer</t>
-  </si>
-  <si>
-    <t>MSM</t>
-  </si>
-  <si>
     <t>boolean</t>
   </si>
   <si>
@@ -67,27 +58,9 @@
     <t>categorical</t>
   </si>
   <si>
-    <t>no HIV</t>
-  </si>
-  <si>
-    <t>early stage HIV</t>
-  </si>
-  <si>
-    <t>late stage HIV</t>
-  </si>
-  <si>
     <t>AIDS</t>
   </si>
   <si>
-    <t>PrEP</t>
-  </si>
-  <si>
-    <t>ART</t>
-  </si>
-  <si>
-    <t>HIV</t>
-  </si>
-  <si>
     <t>race</t>
   </si>
   <si>
@@ -100,28 +73,58 @@
     <t>latinX</t>
   </si>
   <si>
-    <t>asian/pacific islander</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
     <t>not on ART (anti-retroviral therapy)</t>
   </si>
   <si>
-    <t>on ART, adherent</t>
-  </si>
-  <si>
-    <t>was on ART, not adherent</t>
-  </si>
-  <si>
     <t>not on PrEP (pre-exposure prophylaxis)</t>
   </si>
   <si>
-    <t>on PrEP, adherent</t>
-  </si>
-  <si>
-    <t>on PrEP, not adherent</t>
+    <t>age_min</t>
+  </si>
+  <si>
+    <t>age_max</t>
+  </si>
+  <si>
+    <t>maximum age of demographic group</t>
+  </si>
+  <si>
+    <t>minimum age of demographic group</t>
+  </si>
+  <si>
+    <t>uninfected</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>asymptomatic</t>
+  </si>
+  <si>
+    <t>symptomatic</t>
+  </si>
+  <si>
+    <t>on PrEP</t>
+  </si>
+  <si>
+    <t>aware</t>
+  </si>
+  <si>
+    <t>aware of serostatus</t>
+  </si>
+  <si>
+    <t>msm</t>
+  </si>
+  <si>
+    <t>hiv</t>
+  </si>
+  <si>
+    <t>prep</t>
+  </si>
+  <si>
+    <t>art</t>
+  </si>
+  <si>
+    <t>on ART</t>
   </si>
 </sst>
 </file>
@@ -962,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="102" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -992,172 +995,184 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C8">
-        <v>4</v>
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
         <v>0</v>
       </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C16">
-        <v>1</v>
-      </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1165,15 +1180,7 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>